<commit_message>
final commit for sprint 5
</commit_message>
<xml_diff>
--- a/Sprint 5/robbie_robots.xlsx
+++ b/Sprint 5/robbie_robots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="159">
   <si>
     <t>Product Name:</t>
   </si>
@@ -486,6 +486,27 @@
   </si>
   <si>
     <t>dlr</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>tab</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>create new</t>
+  </si>
+  <si>
+    <t>add a window</t>
+  </si>
+  <si>
+    <t>add tabs on top of window</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -797,11 +818,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-58957936"/>
-        <c:axId val="-58952288"/>
+        <c:axId val="-211694400"/>
+        <c:axId val="-211698432"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-58952288"/>
+        <c:axId val="-211698432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,12 +877,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-58957936"/>
+        <c:crossAx val="-211694400"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-58957936"/>
+        <c:axId val="-211694400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +927,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-58952288"/>
+        <c:crossAx val="-211698432"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1029,11 +1050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-59363888"/>
-        <c:axId val="63220832"/>
+        <c:axId val="-310731248"/>
+        <c:axId val="-310734640"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="63220832"/>
+        <c:axId val="-310734640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,12 +1109,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-59363888"/>
+        <c:crossAx val="-310731248"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-59363888"/>
+        <c:axId val="-310731248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63220832"/>
+        <c:crossAx val="-310734640"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1182,7 +1203,7 @@
         <xdr:cNvPr id="2" name="shape">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A45E3298-E1E8-4846-A62C-3754AF100B49}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45E3298-E1E8-4846-A62C-3754AF100B49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1213,7 +1234,7 @@
         <xdr:cNvPr id="2" name="shape">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8FDD3507-7D2C-45CE-AE42-EA1FCB3F7557}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDD3507-7D2C-45CE-AE42-EA1FCB3F7557}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1533,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1658,7 +1679,9 @@
         <v>2</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1"/>
@@ -1670,7 +1693,9 @@
         <v>3</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="1"/>
@@ -1682,7 +1707,9 @@
         <v>4</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>1001246436</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1"/>
@@ -2767,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3006,6 +3033,48 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
   <headerFooter>

</xml_diff>